<commit_message>
fixed the salinity section on some sides
</commit_message>
<xml_diff>
--- a/data/journal_data1.xlsx
+++ b/data/journal_data1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Noah\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Thesis\DATA\Stream Data Complete\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5859CF54-C5B5-44C6-A452-EF471B47AAFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A4E8E9F-9141-4A62-A12E-5EB9FECCB1F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="6" xr2:uid="{C9B4EEB1-E51D-40BE-941B-1657E5511554}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{C9B4EEB1-E51D-40BE-941B-1657E5511554}"/>
   </bookViews>
   <sheets>
     <sheet name="bouge_jour_1" sheetId="1" r:id="rId1"/>
@@ -551,8 +551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90E22DB4-D267-4555-BAC8-19DB31C3EC0D}">
   <dimension ref="A1:AK2"/>
   <sheetViews>
-    <sheetView topLeftCell="Z1" workbookViewId="0">
-      <selection activeCell="AK2" sqref="AK2"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -699,16 +699,16 @@
         <v>8.1333333333333329</v>
       </c>
       <c r="I2" s="1">
-        <v>0.2</v>
+        <v>0.02</v>
       </c>
       <c r="J2" s="1">
-        <v>0.2</v>
+        <v>0.02</v>
       </c>
       <c r="K2" s="1">
-        <v>0.2</v>
+        <v>0.02</v>
       </c>
       <c r="L2" s="1">
-        <v>0.20000000000000004</v>
+        <v>0.02</v>
       </c>
       <c r="M2" s="1">
         <v>1.44E-2</v>
@@ -795,7 +795,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BC998CA-3917-41C1-9D62-AAE12DFC3F9E}">
   <dimension ref="A1:AK2"/>
   <sheetViews>
-    <sheetView topLeftCell="AF1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <selection activeCell="AM3" sqref="AM3"/>
     </sheetView>
   </sheetViews>
@@ -2015,7 +2015,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D91162CD-2744-4E89-B1FF-D9BDAEC82570}">
   <dimension ref="A1:AK2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
+    <sheetView topLeftCell="AE1" workbookViewId="0">
       <selection activeCell="AK2" sqref="AK2"/>
     </sheetView>
   </sheetViews>

</xml_diff>